<commit_message>
Worked on MPW-483 (finalized)
</commit_message>
<xml_diff>
--- a/app/files/samples/products-bonus-sample.xlsx
+++ b/app/files/samples/products-bonus-sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elemenopi\Desktop\Aumet\aumet-marketplace-web\app\files\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E14F06F-59BB-4316-91C4-F8D60AC6052D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF765D0D-111F-497D-B04C-BE09184E190A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{270CAEAE-2440-4052-B598-267330C3A3A1}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{270CAEAE-2440-4052-B598-267330C3A3A1}"/>
   </bookViews>
   <sheets>
     <sheet name="User Input" sheetId="1" r:id="rId1"/>
@@ -469,7 +469,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V2507"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -8044,7 +8044,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1" xr:uid="{5B361486-FAF8-48A0-AE83-2391F64120DB}"/>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F2505" xr:uid="{AAB385A3-4DB3-4C4E-A3B9-9FEF7F611BD2}">
       <formula1>1</formula1>
@@ -8052,7 +8052,10 @@
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E2505 B3:B2505" xr:uid="{495629A8-57D5-4E52-AA56-9AB065592864}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:D2505" xr:uid="{47E63748-57D0-411F-8AA7-E1CED5715774}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C2505" xr:uid="{47E63748-57D0-411F-8AA7-E1CED5715774}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D2505" xr:uid="{3EB9167E-56B2-4D31-8AED-E78FD51BC0E4}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -8065,7 +8068,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E2505"/>
   <sheetViews>
-    <sheetView showZeros="0" workbookViewId="0">
+    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>